<commit_message>
LiDar measurements and analysis
</commit_message>
<xml_diff>
--- a/0100_Research/0120_Prototypes/0122_LiDarLitev4/TestProtocol_LIDARLitev4.xlsx
+++ b/0100_Research/0120_Prototypes/0122_LiDarLitev4/TestProtocol_LIDARLitev4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6e675ddd269f32ab/Documents/3e/PGA/git/LoRaSnow/0100_Research/0120_Prototypes/0122_LiDarLitev4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="268" documentId="11_AD4D9D64A577C15A4A5418AA809858665BDEDD8C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E93EBF37-BCA5-4DFC-8AC3-9E66D984CB4E}"/>
+  <xr:revisionPtr revIDLastSave="279" documentId="11_AD4D9D64A577C15A4A5418AA809858665BDEDD8C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BF6F406-160C-4683-B045-BBA0850491ED}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6045" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests Result " sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="53">
   <si>
     <t>Sensor under test</t>
   </si>
@@ -182,6 +182,18 @@
   </si>
   <si>
     <t>After a quick test on Arduino, a programm was developped on a STM32F746G-DISCO board in order to use a more powerful processor. The sensor outputs distance measurments without any problem.</t>
+  </si>
+  <si>
+    <t>The error characteristic was done on a scale from 20cm to 600cm. Turned out the sensor can't properly measure anything after 300cm. Between 0cm and 300cm, we can expect an error between 1cm and 5cm. We now need to know if this error is constant in temperature and between different sets or not.</t>
+  </si>
+  <si>
+    <t>Further measurement showed that the sensor has a typical error of +-2cm.</t>
+  </si>
+  <si>
+    <t>The test was done in a temperature-controlled environment with temperature from -15°C to 40°C. Results showed that the sensor is almost not disturbed by the temperature and stay in its +-2cm error from the real distance.</t>
+  </si>
+  <si>
+    <t>The sensor pass the test and can be reliably used at various temperatures.</t>
   </si>
 </sst>
 </file>
@@ -986,8 +998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="13.5" x14ac:dyDescent="0.45"/>
@@ -1018,7 +1030,7 @@
       </c>
       <c r="C2" s="14">
         <f>COUNTIF(C3:C986,"Success")/COUNTA(C3:C986)</f>
-        <v>0.125</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.45">
@@ -1114,20 +1126,24 @@
       </c>
       <c r="C14" s="9"/>
     </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A15" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="8"/>
+      <c r="B15" s="17" t="s">
+        <v>49</v>
+      </c>
       <c r="C15" s="9"/>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A16" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="11"/>
+      <c r="B16" s="18" t="s">
+        <v>50</v>
+      </c>
       <c r="C16" s="12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1167,20 +1183,20 @@
       </c>
       <c r="C21" s="9"/>
     </row>
-    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A22" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="8"/>
+      <c r="B22" s="17"/>
       <c r="C22" s="9"/>
     </row>
-    <row r="23" spans="1:3" ht="15" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A23" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="11"/>
+      <c r="B23" s="18"/>
       <c r="C23" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1220,20 +1236,20 @@
       </c>
       <c r="C28" s="9"/>
     </row>
-    <row r="29" spans="1:3" ht="15" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A29" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="8"/>
+      <c r="B29" s="17"/>
       <c r="C29" s="9"/>
     </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A30" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="11"/>
+      <c r="B30" s="18"/>
       <c r="C30" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1273,20 +1289,24 @@
       </c>
       <c r="C35" s="9"/>
     </row>
-    <row r="36" spans="1:3" ht="15" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:3" ht="46.15" x14ac:dyDescent="0.45">
       <c r="A36" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="8"/>
+      <c r="B36" s="17" t="s">
+        <v>51</v>
+      </c>
       <c r="C36" s="9"/>
     </row>
-    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A37" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="11"/>
+      <c r="B37" s="18" t="s">
+        <v>52</v>
+      </c>
       <c r="C37" s="12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1326,18 +1346,18 @@
       </c>
       <c r="C42" s="9"/>
     </row>
-    <row r="43" spans="1:3" ht="15" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A43" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B43" s="8"/>
+      <c r="B43" s="17"/>
       <c r="C43" s="9"/>
     </row>
-    <row r="44" spans="1:3" ht="15" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A44" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="11"/>
+      <c r="B44" s="18"/>
       <c r="C44" s="12" t="s">
         <v>12</v>
       </c>
@@ -1379,18 +1399,18 @@
       </c>
       <c r="C49" s="9"/>
     </row>
-    <row r="50" spans="1:3" ht="15" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A50" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B50" s="8"/>
+      <c r="B50" s="17"/>
       <c r="C50" s="9"/>
     </row>
-    <row r="51" spans="1:3" ht="15" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A51" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B51" s="11"/>
+      <c r="B51" s="18"/>
       <c r="C51" s="12" t="s">
         <v>12</v>
       </c>
@@ -1432,18 +1452,18 @@
       </c>
       <c r="C56" s="9"/>
     </row>
-    <row r="57" spans="1:3" ht="15" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A57" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B57" s="8"/>
+      <c r="B57" s="17"/>
       <c r="C57" s="9"/>
     </row>
-    <row r="58" spans="1:3" ht="15" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A58" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B58" s="11"/>
+      <c r="B58" s="18"/>
       <c r="C58" s="12" t="s">
         <v>12</v>
       </c>

</xml_diff>